<commit_message>
Borrar puntos al final de frases en viñetas para versionas Full CV
</commit_message>
<xml_diff>
--- a/ENG/data/award.xlsx
+++ b/ENG/data/award.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV-master\ENG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3C8DCE-8968-4904-81FA-C814C3A3DB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E6DF67-8273-40D8-9F2B-3AEF1B5B15C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
   <si>
     <t>what</t>
   </si>
@@ -127,10 +127,13 @@
     <t>Ig Nobel Prize</t>
   </si>
   <si>
-    <t>For ‘trying to quantify the relationship between different countries’ national income inequality and the average amount of mouth-to-mouth kissing’ (Watkins,, et al., 2019).</t>
-  </si>
-  <si>
     <t>Cambridge, MA, USA.</t>
+  </si>
+  <si>
+    <t>Best overall performance in the MSc</t>
+  </si>
+  <si>
+    <t>For ‘trying to quantify the relationship between different countries’ national income inequality and the average amount of mouth-to-mouth kissing’ (Watkins, et al., 2019)</t>
   </si>
 </sst>
 </file>
@@ -990,7 +993,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,10 +1033,10 @@
         <v>34</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,7 +1132,7 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added further education, and presentations for VRI. Could not recover footer
</commit_message>
<xml_diff>
--- a/ENG/data/award.xlsx
+++ b/ENG/data/award.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV-master\ENG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E6DF67-8273-40D8-9F2B-3AEF1B5B15C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123B81BB-DA5C-4F29-A5DF-24616414A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>what</t>
   </si>
@@ -37,9 +37,6 @@
     <t>why</t>
   </si>
   <si>
-    <t>Colciencias</t>
-  </si>
-  <si>
     <t>Bogota, Colombia</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Liverpool, UK</t>
   </si>
   <si>
-    <t>Best overall performance in the MSc.</t>
-  </si>
-  <si>
     <t>University of Liverpool International Scholarship</t>
   </si>
   <si>
@@ -134,6 +128,9 @@
   </si>
   <si>
     <t>For ‘trying to quantify the relationship between different countries’ national income inequality and the average amount of mouth-to-mouth kissing’ (Watkins, et al., 2019)</t>
+  </si>
+  <si>
+    <t>Minciencias</t>
   </si>
 </sst>
 </file>
@@ -993,7 +990,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,143 +1021,143 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>